<commit_message>
Terminada seccion experimentos en paper
</commit_message>
<xml_diff>
--- a/others/paper/experimentos.xlsx
+++ b/others/paper/experimentos.xlsx
@@ -26,12 +26,6 @@
     <t>Punto Objetivo</t>
   </si>
   <si>
-    <t>Distancia de Aproximación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rango Sonar </t>
-  </si>
-  <si>
     <t>Error Distancia</t>
   </si>
   <si>
@@ -90,13 +84,19 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Distancia Mínima</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ángulo Sonar </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,16 +104,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -121,68 +143,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
@@ -241,15 +226,27 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -267,15 +264,35 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -286,9 +303,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabla15" displayName="Tabla15" ref="B4:H11" totalsRowCount="1">
   <autoFilter ref="B4:H10"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Nro" totalsRowDxfId="15"/>
-    <tableColumn id="2" name="Punto Inicio" dataDxfId="19" totalsRowDxfId="14"/>
-    <tableColumn id="3" name="Punto Objetivo" dataDxfId="18" totalsRowDxfId="13"/>
+    <tableColumn id="1" name="Nro" totalsRowDxfId="17"/>
+    <tableColumn id="2" name="Punto Inicio" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="3" name="Punto Objetivo" dataDxfId="14" totalsRowDxfId="13"/>
     <tableColumn id="6" name="Error Distancia" totalsRowDxfId="12"/>
     <tableColumn id="7" name="Error Ángulo" totalsRowDxfId="11"/>
     <tableColumn id="8" name="Éxito" totalsRowFunction="custom" totalsRowDxfId="10">
@@ -301,16 +318,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="B4:J11" totalsRowCount="1">
-  <autoFilter ref="B4:J10"/>
-  <tableColumns count="9">
-    <tableColumn id="1" name="Nro" totalsRowDxfId="8"/>
-    <tableColumn id="2" name="Punto Inicio" dataDxfId="17" totalsRowDxfId="7"/>
-    <tableColumn id="3" name="Punto Objetivo" dataDxfId="16" totalsRowDxfId="6"/>
-    <tableColumn id="4" name="Distancia de Aproximación" totalsRowDxfId="5"/>
-    <tableColumn id="5" name="Rango Sonar " totalsRowDxfId="4"/>
-    <tableColumn id="6" name="Error Distancia" totalsRowDxfId="3"/>
-    <tableColumn id="7" name="Error Ángulo" totalsRowDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="C6:I13" totalsRowCount="1">
+  <autoFilter ref="C6:I12"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Nro" totalsRowDxfId="6"/>
+    <tableColumn id="2" name="Punto Inicio" dataDxfId="8" totalsRowDxfId="5"/>
+    <tableColumn id="3" name="Punto Objetivo" dataDxfId="7" totalsRowDxfId="4"/>
+    <tableColumn id="4" name="Distancia Mínima" totalsRowDxfId="3"/>
+    <tableColumn id="5" name="Ángulo Sonar " totalsRowDxfId="2"/>
     <tableColumn id="8" name="Éxito" totalsRowFunction="custom" totalsRowDxfId="1">
       <totalsRowFormula>COUNTIF([Éxito],"Si")*100/6</totalsRowFormula>
     </tableColumn>
@@ -607,9 +622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
@@ -621,8 +634,8 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8">
-      <c r="B2" t="s">
-        <v>9</v>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:8">
@@ -636,16 +649,16 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" t="s">
         <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:8">
@@ -653,10 +666,10 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <v>30</v>
@@ -665,7 +678,7 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H5">
         <v>419.17</v>
@@ -676,10 +689,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6">
         <v>30</v>
@@ -688,7 +701,7 @@
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H6">
         <v>417.29</v>
@@ -699,10 +712,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>40</v>
@@ -711,7 +724,7 @@
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H7">
         <v>455.21</v>
@@ -722,10 +735,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E8">
         <v>40</v>
@@ -734,7 +747,7 @@
         <v>4</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H8">
         <v>310.5</v>
@@ -745,10 +758,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E9">
         <v>60</v>
@@ -757,7 +770,7 @@
         <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H9">
         <v>317.64</v>
@@ -768,10 +781,10 @@
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E10" s="2">
         <v>60</v>
@@ -780,7 +793,7 @@
         <v>6</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H10" s="2">
         <v>429.77</v>
@@ -808,238 +821,209 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:J11"/>
+  <dimension ref="C2:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
-      <c r="B2" t="s">
+    <row r="2" spans="3:9">
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9">
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9">
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9">
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="2:10">
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="F7">
+        <v>500</v>
+      </c>
+      <c r="G7">
+        <v>45</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7">
+        <v>540.16999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9">
+      <c r="C8">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>500</v>
+      </c>
+      <c r="G8">
+        <v>55</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8">
+        <v>130.44</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9">
+      <c r="C9">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="D9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9">
+        <v>400</v>
+      </c>
+      <c r="G9">
+        <v>45</v>
+      </c>
+      <c r="H9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9">
+        <v>529.08000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9">
+      <c r="C10">
         <v>4</v>
       </c>
-      <c r="G4" t="s">
+      <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10">
+        <v>400</v>
+      </c>
+      <c r="G10">
+        <v>55</v>
+      </c>
+      <c r="H10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10">
+        <v>383.89</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9">
+      <c r="C11">
         <v>5</v>
       </c>
-      <c r="H4" t="s">
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11">
+        <v>300</v>
+      </c>
+      <c r="G11">
+        <v>45</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9">
+      <c r="C12" s="2">
         <v>6</v>
       </c>
-      <c r="I4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10">
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>500</v>
-      </c>
-      <c r="F5">
-        <v>45</v>
-      </c>
-      <c r="G5">
-        <v>30</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5">
-        <v>540.16999999999996</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10">
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6">
-        <v>500</v>
-      </c>
-      <c r="F6">
+      <c r="D12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="2">
+        <v>300</v>
+      </c>
+      <c r="G12">
         <v>55</v>
       </c>
-      <c r="G6">
-        <v>30</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6">
-        <v>130.44</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7">
-        <v>400</v>
-      </c>
-      <c r="F7">
-        <v>45</v>
-      </c>
-      <c r="G7">
-        <v>30</v>
-      </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
-      <c r="I7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7">
-        <v>529.08000000000004</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10">
-      <c r="B8">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8">
-        <v>400</v>
-      </c>
-      <c r="F8">
-        <v>55</v>
-      </c>
-      <c r="G8">
-        <v>30</v>
-      </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-      <c r="I8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8">
-        <v>383.89</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10">
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9">
-        <v>300</v>
-      </c>
-      <c r="F9">
-        <v>45</v>
-      </c>
-      <c r="G9">
-        <v>30</v>
-      </c>
-      <c r="H9">
-        <v>2</v>
-      </c>
-      <c r="I9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="2">
-        <v>6</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="H12" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="2">
-        <v>300</v>
-      </c>
-      <c r="F10">
-        <v>55</v>
-      </c>
-      <c r="G10">
-        <v>30</v>
-      </c>
-      <c r="H10">
-        <v>2</v>
-      </c>
-      <c r="I10" t="s">
-        <v>24</v>
-      </c>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="2:10">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2">
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="3:9">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2">
         <f>COUNTIF([Éxito],"Si")*100/6</f>
         <v>66.666666666666671</v>
       </c>
-      <c r="J11" s="2"/>
+      <c r="I13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>